<commit_message>
valido si las fotos vienen nulas and informe tecnico modo prueba
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -136,22 +136,25 @@
     <t>Cambio de Caps (60cu)</t>
   </si>
   <si>
+    <t>Marcado de Caps</t>
+  </si>
+  <si>
     <t>30 May, 2017, 2:58 pm</t>
   </si>
   <si>
-    <t>Marcado de Caps</t>
+    <t>Marcado de Caps2</t>
   </si>
   <si>
-    <t>Marcado de Caps 3</t>
+    <t>Marcado de Caps3</t>
   </si>
   <si>
-    <t>Marcado de Caps 4</t>
+    <t>Marcado de Caps4</t>
   </si>
   <si>
-    <t>Marcado de Caps 5</t>
+    <t>Marcado de Caps5</t>
   </si>
   <si>
-    <t>Marcado de Caps 6</t>
+    <t>Marcado de Caps6</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -166,37 +169,37 @@
     <t>1.-</t>
   </si>
   <si>
-    <t>1: Pf</t>
+    <t>Marcado de Caps: Pf</t>
   </si>
   <si>
     <t>2.-</t>
   </si>
   <si>
-    <t>Marcado de Caps: Pf</t>
+    <t>Marcado de Caps2: Pf</t>
   </si>
   <si>
     <t>3.-</t>
   </si>
   <si>
-    <t>Marcado de Caps 3: Pf</t>
+    <t>Marcado de Caps3: Pf</t>
   </si>
   <si>
     <t>4.-</t>
   </si>
   <si>
-    <t>Marcado de Caps 4: Pf</t>
+    <t>Marcado de Caps4: Pf</t>
   </si>
   <si>
     <t>5.-</t>
   </si>
   <si>
-    <t>Marcado de Caps 5: Pf</t>
+    <t>Marcado de Caps5: Pf</t>
   </si>
   <si>
     <t>6.-</t>
   </si>
   <si>
-    <t>Marcado de Caps 6: Pf</t>
+    <t>Marcado de Caps6: Pf</t>
   </si>
   <si>
     <t>REGISTRO FOTOGRÁFICO</t>
@@ -217,10 +220,19 @@
     <t>Foto 4:</t>
   </si>
   <si>
+    <t>leyenda 4</t>
+  </si>
+  <si>
     <t>Foto 5:</t>
   </si>
   <si>
+    <t>leyenda 5</t>
+  </si>
+  <si>
     <t>Foto 6:</t>
+  </si>
+  <si>
+    <t>leyenda 6</t>
   </si>
 </sst>
 </file>
@@ -1164,11 +1176,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Foto Trabajo 1" descr="Trabajo 1"/>
@@ -1194,11 +1206,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="6" name="Foto Trabajo 2" descr="Trabajo 2"/>
@@ -1224,11 +1236,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="7" name="Foto Trabajo 3" descr="Trabajo 3"/>
@@ -1254,11 +1266,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="8" name="Foto Trabajo 4" descr="Trabajo 4"/>
@@ -1284,11 +1296,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="9" name="Foto Trabajo 5" descr="Trabajo 5"/>
@@ -1314,11 +1326,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:ext cx="2466975" cy="3286125"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="10" name="Foto Trabajo 6" descr="Trabajo 6"/>
@@ -22286,8 +22298,8 @@
       <c r="B21" s="43"/>
       <c r="C21" s="44"/>
       <c r="D21" s="39"/>
-      <c r="E21" s="39">
-        <v>1</v>
+      <c r="E21" s="39" t="s">
+        <v>34</v>
       </c>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
@@ -22312,7 +22324,7 @@
       <c r="Z21" s="39"/>
       <c r="AA21" s="39"/>
       <c r="AB21" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC21" s="45"/>
       <c r="AD21" s="45"/>
@@ -22320,7 +22332,7 @@
       <c r="AF21" s="45"/>
       <c r="AG21" s="45"/>
       <c r="AH21" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI21" s="45"/>
       <c r="AJ21" s="45"/>
@@ -23321,7 +23333,7 @@
       <c r="C22" s="44"/>
       <c r="D22" s="39"/>
       <c r="E22" s="39" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
@@ -23346,7 +23358,7 @@
       <c r="Z22" s="39"/>
       <c r="AA22" s="39"/>
       <c r="AB22" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC22" s="47"/>
       <c r="AD22" s="47"/>
@@ -23354,7 +23366,7 @@
       <c r="AF22" s="47"/>
       <c r="AG22" s="47"/>
       <c r="AH22" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI22" s="47"/>
       <c r="AJ22" s="47"/>
@@ -24355,7 +24367,7 @@
       <c r="C23" s="44"/>
       <c r="D23" s="39"/>
       <c r="E23" s="39" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
@@ -24380,7 +24392,7 @@
       <c r="Z23" s="39"/>
       <c r="AA23" s="39"/>
       <c r="AB23" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
@@ -24388,7 +24400,7 @@
       <c r="AF23" s="47"/>
       <c r="AG23" s="47"/>
       <c r="AH23" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI23" s="47"/>
       <c r="AJ23" s="47"/>
@@ -25388,7 +25400,7 @@
       <c r="C24" s="44"/>
       <c r="D24" s="39"/>
       <c r="E24" s="39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
@@ -25413,7 +25425,7 @@
       <c r="Z24" s="39"/>
       <c r="AA24" s="39"/>
       <c r="AB24" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
@@ -25421,7 +25433,7 @@
       <c r="AF24" s="47"/>
       <c r="AG24" s="47"/>
       <c r="AH24" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI24" s="47"/>
       <c r="AJ24" s="47"/>
@@ -25472,7 +25484,7 @@
       <c r="C25" s="44"/>
       <c r="D25" s="39"/>
       <c r="E25" s="39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F25" s="39"/>
       <c r="G25" s="39"/>
@@ -25497,7 +25509,7 @@
       <c r="Z25" s="39"/>
       <c r="AA25" s="39"/>
       <c r="AB25" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC25" s="47"/>
       <c r="AD25" s="47"/>
@@ -25505,7 +25517,7 @@
       <c r="AF25" s="47"/>
       <c r="AG25" s="47"/>
       <c r="AH25" s="47" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI25" s="47"/>
       <c r="AJ25" s="47"/>
@@ -25557,7 +25569,7 @@
       <c r="C26" s="44"/>
       <c r="D26" s="39"/>
       <c r="E26" s="39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
@@ -25582,7 +25594,7 @@
       <c r="Z26" s="39"/>
       <c r="AA26" s="39"/>
       <c r="AB26" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AC26" s="45"/>
       <c r="AD26" s="45"/>
@@ -25590,7 +25602,7 @@
       <c r="AF26" s="45"/>
       <c r="AG26" s="45"/>
       <c r="AH26" s="45" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AI26" s="45"/>
       <c r="AJ26" s="45"/>
@@ -43004,7 +43016,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="10"/>
       <c r="B43" s="55" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
@@ -44032,7 +44044,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="10"/>
       <c r="B44" s="24" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -44069,7 +44081,7 @@
       <c r="AI44" s="24"/>
       <c r="AJ44" s="24"/>
       <c r="AK44" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AL44" s="25"/>
       <c r="AM44" s="25"/>
@@ -45063,10 +45075,10 @@
       <c r="A45" s="10"/>
       <c r="B45" s="56"/>
       <c r="C45" s="57" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D45" s="57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E45" s="57"/>
       <c r="F45" s="58"/>
@@ -46093,10 +46105,10 @@
       <c r="A46" s="10"/>
       <c r="B46" s="56"/>
       <c r="C46" s="57" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D46" s="57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E46" s="57"/>
       <c r="F46" s="58"/>
@@ -47123,10 +47135,10 @@
       <c r="A47" s="10"/>
       <c r="B47" s="56"/>
       <c r="C47" s="60" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D47" s="60" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E47" s="60"/>
       <c r="F47" s="60"/>
@@ -48153,10 +48165,10 @@
       <c r="A48" s="10"/>
       <c r="B48" s="56"/>
       <c r="C48" s="60" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D48" s="60" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E48" s="60"/>
       <c r="F48" s="60"/>
@@ -49183,10 +49195,10 @@
       <c r="A49" s="10"/>
       <c r="B49" s="56"/>
       <c r="C49" s="60" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D49" s="60" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
@@ -50213,10 +50225,10 @@
       <c r="A50" s="10"/>
       <c r="B50" s="56"/>
       <c r="C50" s="60" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D50" s="60" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E50" s="60"/>
       <c r="F50" s="60"/>
@@ -51242,7 +51254,7 @@
     <row r="51" spans="1:1025" customHeight="1" ht="15">
       <c r="A51" s="10"/>
       <c r="B51" s="62" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C51" s="62"/>
       <c r="D51" s="62"/>
@@ -52270,11 +52282,11 @@
     <row r="52" spans="1:1025" customHeight="1" ht="13.25">
       <c r="A52" s="10"/>
       <c r="B52" s="63" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C52" s="63"/>
       <c r="D52" s="64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E52" s="64"/>
       <c r="F52" s="64"/>
@@ -52288,11 +52300,11 @@
       <c r="N52" s="64"/>
       <c r="O52" s="64"/>
       <c r="P52" s="65" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q52" s="65"/>
       <c r="R52" s="64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S52" s="64"/>
       <c r="T52" s="64"/>
@@ -52306,11 +52318,11 @@
       <c r="AB52" s="64"/>
       <c r="AC52" s="64"/>
       <c r="AD52" s="65" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AE52" s="65"/>
       <c r="AF52" s="64" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AG52" s="64"/>
       <c r="AH52" s="64"/>
@@ -66690,11 +66702,11 @@
     <row r="67" spans="1:1025" customHeight="1" ht="15">
       <c r="A67"/>
       <c r="B67" s="63" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C67" s="63"/>
       <c r="D67" s="64" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E67" s="64"/>
       <c r="F67" s="64"/>
@@ -66708,11 +66720,11 @@
       <c r="N67" s="64"/>
       <c r="O67" s="64"/>
       <c r="P67" s="65" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="Q67" s="65"/>
       <c r="R67" s="64" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="S67" s="64"/>
       <c r="T67" s="64"/>
@@ -66726,11 +66738,11 @@
       <c r="AB67" s="64"/>
       <c r="AC67" s="64"/>
       <c r="AD67" s="65" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AE67" s="65"/>
       <c r="AF67" s="71" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="AG67" s="71"/>
       <c r="AH67" s="71"/>

</xml_diff>

<commit_message>
Add filter desde and avance
</commit_message>
<xml_diff>
--- a/ReportOut.xlsx
+++ b/ReportOut.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>Fabricación, Montaje, Mantención y Reparación</t>
   </si>
@@ -127,28 +127,61 @@
     <t>Avance</t>
   </si>
   <si>
-    <t>Cambio de Caps (70cu)</t>
+    <t>dambio de Caps (60cu)</t>
   </si>
   <si>
-    <t>Marcado de Caps2</t>
+    <t>arcado de Caps9</t>
   </si>
   <si>
-    <t>14 May, 2017, 1:58 pm</t>
+    <t>16 May, 2017, 12:14 am</t>
   </si>
   <si>
-    <t>15 May, 2017, 3:58 pm</t>
+    <t>18 May, 2017, 3:58 pm</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>Marcado de Caps3</t>
+    <t>arcado de Caps10</t>
   </si>
   <si>
-    <t>16 May, 2017, 1:58 pm</t>
+    <t>16 May, 2017, 12:19 am</t>
   </si>
   <si>
-    <t>18 May, 2017, 3:58 pm</t>
+    <t>18 May, 2017, 1:58 am</t>
+  </si>
+  <si>
+    <t>arcado de Caps1</t>
+  </si>
+  <si>
+    <t>16 May, 2017, 2:58 am</t>
+  </si>
+  <si>
+    <t>arcado de Caps4</t>
+  </si>
+  <si>
+    <t>arcado de Caps5</t>
+  </si>
+  <si>
+    <t>arcado de Caps6</t>
+  </si>
+  <si>
+    <t>arcado de Caps7</t>
+  </si>
+  <si>
+    <t>farcado de Caps1</t>
+  </si>
+  <si>
+    <t>Cambio de Caps (60cu)</t>
+  </si>
+  <si>
+    <t>zarcado de Caps1</t>
+  </si>
+  <si>
+    <t>arcado de Caps8</t>
+  </si>
+  <si>
+    <t>16 May, 2017, 12:14 pm</t>
   </si>
   <si>
     <t>PARA DETALLES VER EN ESQUEMAS PROXIMA PAGINA</t>
@@ -1170,6 +1203,126 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Foto Trabajo 1" descr="Trabajo 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Foto Trabajo 1" descr="Trabajo 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Foto Trabajo 1" descr="Trabajo 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="0"/>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4381500" cy="3286125"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Foto Trabajo 1" descr="Trabajo 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -24195,8 +24348,12 @@
       <c r="A23"/>
       <c r="B23" s="43"/>
       <c r="C23" s="44"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
+      <c r="D23" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
@@ -24219,19 +24376,25 @@
       <c r="Y23" s="39"/>
       <c r="Z23" s="39"/>
       <c r="AA23" s="39"/>
-      <c r="AB23" s="47"/>
+      <c r="AB23" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
       <c r="AE23" s="47"/>
       <c r="AF23" s="47"/>
       <c r="AG23" s="47"/>
-      <c r="AH23" s="47"/>
+      <c r="AH23" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="AI23" s="47"/>
       <c r="AJ23" s="47"/>
       <c r="AK23" s="47"/>
       <c r="AL23" s="47"/>
       <c r="AM23" s="47"/>
-      <c r="AN23" s="42"/>
+      <c r="AN23" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO23" s="42"/>
       <c r="AP23" s="42"/>
       <c r="AQ23" s="42"/>
@@ -25220,8 +25383,12 @@
     <row r="24" spans="1:1025" customHeight="1" ht="15" s="10" customFormat="1">
       <c r="B24" s="43"/>
       <c r="C24" s="44"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>41</v>
+      </c>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
@@ -25244,19 +25411,25 @@
       <c r="Y24" s="39"/>
       <c r="Z24" s="39"/>
       <c r="AA24" s="39"/>
-      <c r="AB24" s="47"/>
+      <c r="AB24" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
       <c r="AE24" s="47"/>
       <c r="AF24" s="47"/>
       <c r="AG24" s="47"/>
-      <c r="AH24" s="47"/>
+      <c r="AH24" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="AI24" s="47"/>
       <c r="AJ24" s="47"/>
       <c r="AK24" s="47"/>
       <c r="AL24" s="47"/>
       <c r="AM24" s="47"/>
-      <c r="AN24" s="42"/>
+      <c r="AN24" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO24" s="42"/>
       <c r="AP24" s="42"/>
       <c r="AQ24" s="42"/>
@@ -25296,8 +25469,12 @@
     <row r="25" spans="1:1025" customHeight="1" ht="15" s="10" customFormat="1">
       <c r="B25" s="43"/>
       <c r="C25" s="44"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
+      <c r="D25" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="39" t="s">
+        <v>42</v>
+      </c>
       <c r="F25" s="39"/>
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
@@ -25320,19 +25497,25 @@
       <c r="Y25" s="39"/>
       <c r="Z25" s="39"/>
       <c r="AA25" s="39"/>
-      <c r="AB25" s="47"/>
+      <c r="AB25" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="AC25" s="47"/>
       <c r="AD25" s="47"/>
       <c r="AE25" s="47"/>
       <c r="AF25" s="47"/>
       <c r="AG25" s="47"/>
-      <c r="AH25" s="47"/>
+      <c r="AH25" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="AI25" s="47"/>
       <c r="AJ25" s="47"/>
       <c r="AK25" s="47"/>
       <c r="AL25" s="47"/>
       <c r="AM25" s="47"/>
-      <c r="AN25" s="42"/>
+      <c r="AN25" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO25" s="42"/>
       <c r="AP25" s="42"/>
       <c r="AQ25" s="42"/>
@@ -25373,8 +25556,12 @@
       <c r="A26" s="10"/>
       <c r="B26" s="43"/>
       <c r="C26" s="44"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
+      <c r="D26" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>43</v>
+      </c>
       <c r="F26" s="39"/>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
@@ -25397,19 +25584,25 @@
       <c r="Y26" s="39"/>
       <c r="Z26" s="39"/>
       <c r="AA26" s="39"/>
-      <c r="AB26" s="45"/>
+      <c r="AB26" s="45" t="s">
+        <v>40</v>
+      </c>
       <c r="AC26" s="45"/>
       <c r="AD26" s="45"/>
       <c r="AE26" s="45"/>
       <c r="AF26" s="45"/>
       <c r="AG26" s="45"/>
-      <c r="AH26" s="45"/>
+      <c r="AH26" s="45" t="s">
+        <v>34</v>
+      </c>
       <c r="AI26" s="45"/>
       <c r="AJ26" s="45"/>
       <c r="AK26" s="45"/>
       <c r="AL26" s="45"/>
       <c r="AM26" s="45"/>
-      <c r="AN26" s="46"/>
+      <c r="AN26" s="46" t="s">
+        <v>35</v>
+      </c>
       <c r="AO26" s="46"/>
       <c r="AP26" s="46"/>
       <c r="AQ26" s="46"/>
@@ -26399,8 +26592,12 @@
       <c r="A27" s="10"/>
       <c r="B27" s="43"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
+      <c r="D27" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>44</v>
+      </c>
       <c r="F27" s="39"/>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
@@ -26423,19 +26620,25 @@
       <c r="Y27" s="39"/>
       <c r="Z27" s="39"/>
       <c r="AA27" s="39"/>
-      <c r="AB27" s="47"/>
+      <c r="AB27" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="AC27" s="47"/>
       <c r="AD27" s="47"/>
       <c r="AE27" s="47"/>
       <c r="AF27" s="47"/>
       <c r="AG27" s="47"/>
-      <c r="AH27" s="47"/>
+      <c r="AH27" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="AI27" s="47"/>
       <c r="AJ27" s="47"/>
       <c r="AK27" s="47"/>
       <c r="AL27" s="47"/>
       <c r="AM27" s="47"/>
-      <c r="AN27" s="42"/>
+      <c r="AN27" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO27" s="42"/>
       <c r="AP27" s="42"/>
       <c r="AQ27" s="42"/>
@@ -27425,8 +27628,12 @@
       <c r="A28" s="10"/>
       <c r="B28" s="43"/>
       <c r="C28" s="44"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
+      <c r="D28" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>45</v>
+      </c>
       <c r="F28" s="39"/>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
@@ -27449,19 +27656,25 @@
       <c r="Y28" s="39"/>
       <c r="Z28" s="39"/>
       <c r="AA28" s="39"/>
-      <c r="AB28" s="45"/>
+      <c r="AB28" s="45" t="s">
+        <v>40</v>
+      </c>
       <c r="AC28" s="45"/>
       <c r="AD28" s="45"/>
       <c r="AE28" s="45"/>
       <c r="AF28" s="45"/>
       <c r="AG28" s="45"/>
-      <c r="AH28" s="45"/>
+      <c r="AH28" s="45" t="s">
+        <v>34</v>
+      </c>
       <c r="AI28" s="45"/>
       <c r="AJ28" s="45"/>
       <c r="AK28" s="45"/>
       <c r="AL28" s="45"/>
       <c r="AM28" s="45"/>
-      <c r="AN28" s="46"/>
+      <c r="AN28" s="46" t="s">
+        <v>35</v>
+      </c>
       <c r="AO28" s="46"/>
       <c r="AP28" s="46"/>
       <c r="AQ28" s="46"/>
@@ -28451,8 +28664,12 @@
       <c r="A29" s="10"/>
       <c r="B29" s="43"/>
       <c r="C29" s="44"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
+      <c r="D29" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="F29" s="39"/>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
@@ -28475,19 +28692,25 @@
       <c r="Y29" s="39"/>
       <c r="Z29" s="39"/>
       <c r="AA29" s="39"/>
-      <c r="AB29" s="47"/>
+      <c r="AB29" s="47" t="s">
+        <v>40</v>
+      </c>
       <c r="AC29" s="47"/>
       <c r="AD29" s="47"/>
       <c r="AE29" s="47"/>
       <c r="AF29" s="47"/>
       <c r="AG29" s="47"/>
-      <c r="AH29" s="47"/>
+      <c r="AH29" s="47" t="s">
+        <v>34</v>
+      </c>
       <c r="AI29" s="47"/>
       <c r="AJ29" s="47"/>
       <c r="AK29" s="47"/>
       <c r="AL29" s="47"/>
       <c r="AM29" s="47"/>
-      <c r="AN29" s="42"/>
+      <c r="AN29" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO29" s="42"/>
       <c r="AP29" s="42"/>
       <c r="AQ29" s="42"/>
@@ -29477,8 +29700,12 @@
       <c r="A30" s="10"/>
       <c r="B30" s="43"/>
       <c r="C30" s="44"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+      <c r="D30" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>48</v>
+      </c>
       <c r="F30" s="39"/>
       <c r="G30" s="39"/>
       <c r="H30" s="39"/>
@@ -29501,19 +29728,25 @@
       <c r="Y30" s="39"/>
       <c r="Z30" s="39"/>
       <c r="AA30" s="39"/>
-      <c r="AB30" s="47"/>
+      <c r="AB30" s="47" t="s">
+        <v>49</v>
+      </c>
       <c r="AC30" s="47"/>
       <c r="AD30" s="47"/>
       <c r="AE30" s="47"/>
       <c r="AF30" s="47"/>
       <c r="AG30" s="47"/>
-      <c r="AH30" s="48"/>
+      <c r="AH30" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="AI30" s="48"/>
       <c r="AJ30" s="48"/>
       <c r="AK30" s="48"/>
       <c r="AL30" s="48"/>
       <c r="AM30" s="48"/>
-      <c r="AN30" s="42"/>
+      <c r="AN30" s="42" t="s">
+        <v>35</v>
+      </c>
       <c r="AO30" s="42"/>
       <c r="AP30" s="42"/>
       <c r="AQ30" s="42"/>
@@ -42814,7 +43047,7 @@
     <row r="43" spans="1:1025" customHeight="1" ht="15">
       <c r="A43" s="10"/>
       <c r="B43" s="55" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C43" s="55"/>
       <c r="D43" s="55"/>
@@ -43842,7 +44075,7 @@
     <row r="44" spans="1:1025" customHeight="1" ht="15">
       <c r="A44" s="10"/>
       <c r="B44" s="24" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="24"/>
@@ -43879,7 +44112,7 @@
       <c r="AI44" s="24"/>
       <c r="AJ44" s="24"/>
       <c r="AK44" s="25" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AL44" s="25"/>
       <c r="AM44" s="25"/>
@@ -44873,7 +45106,7 @@
       <c r="A45" s="10"/>
       <c r="B45" s="56"/>
       <c r="C45" s="57" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D45" s="57"/>
       <c r="E45" s="57"/>
@@ -45901,7 +46134,7 @@
       <c r="A46" s="10"/>
       <c r="B46" s="56"/>
       <c r="C46" s="57" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D46" s="57"/>
       <c r="E46" s="57"/>
@@ -46929,7 +47162,7 @@
       <c r="A47" s="10"/>
       <c r="B47" s="56"/>
       <c r="C47" s="57" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D47" s="57"/>
       <c r="E47" s="57"/>
@@ -47956,7 +48189,7 @@
     <row r="48" spans="1:1025" customHeight="1" ht="15">
       <c r="A48" s="10"/>
       <c r="B48" s="60" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="C48" s="60"/>
       <c r="D48" s="60"/>
@@ -48984,11 +49217,11 @@
     <row r="49" spans="1:1025" customHeight="1" ht="13.35">
       <c r="A49" s="10"/>
       <c r="B49" s="61" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C49" s="61"/>
       <c r="D49" s="62" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E49" s="62"/>
       <c r="F49" s="62"/>
@@ -49002,11 +49235,11 @@
       <c r="N49" s="62"/>
       <c r="O49" s="62"/>
       <c r="P49" s="63" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="Q49" s="63"/>
       <c r="R49" s="62" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="S49" s="62"/>
       <c r="T49" s="62"/>
@@ -49020,10 +49253,12 @@
       <c r="AB49" s="62"/>
       <c r="AC49" s="62"/>
       <c r="AD49" s="63" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AE49" s="63"/>
-      <c r="AF49" s="62"/>
+      <c r="AF49" s="62" t="s">
+        <v>58</v>
+      </c>
       <c r="AG49" s="62"/>
       <c r="AH49" s="62"/>
       <c r="AI49" s="62"/>
@@ -63402,10 +63637,12 @@
     <row r="64" spans="1:1025" customHeight="1" ht="15">
       <c r="A64"/>
       <c r="B64" s="61" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C64" s="61"/>
-      <c r="D64" s="62"/>
+      <c r="D64" s="62" t="s">
+        <v>58</v>
+      </c>
       <c r="E64" s="62"/>
       <c r="F64" s="62"/>
       <c r="G64" s="62"/>
@@ -63418,10 +63655,12 @@
       <c r="N64" s="62"/>
       <c r="O64" s="62"/>
       <c r="P64" s="63" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="Q64" s="63"/>
-      <c r="R64" s="62"/>
+      <c r="R64" s="62" t="s">
+        <v>58</v>
+      </c>
       <c r="S64" s="62"/>
       <c r="T64" s="62"/>
       <c r="U64" s="62"/>
@@ -63434,10 +63673,12 @@
       <c r="AB64" s="62"/>
       <c r="AC64" s="62"/>
       <c r="AD64" s="63" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="AE64" s="63"/>
-      <c r="AF64" s="69"/>
+      <c r="AF64" s="69" t="s">
+        <v>58</v>
+      </c>
       <c r="AG64" s="69"/>
       <c r="AH64" s="69"/>
       <c r="AI64" s="69"/>

</xml_diff>